<commit_message>
commit process animals done and working
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexandruRotar\Documents\GitHub\API-ANIMALS-PERFORMER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9528F7-BD23-4389-9802-9731D5E48DE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F2D4B6-3CA3-42D7-8E0B-568123B90728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2145" windowWidth="18030" windowHeight="12540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -172,6 +172,51 @@
   </si>
   <si>
     <t>C:\Users\AlexandruRotar\Desktop\API Output Report</t>
+  </si>
+  <si>
+    <t>listOfAnimals</t>
+  </si>
+  <si>
+    <t>cat;dog</t>
+  </si>
+  <si>
+    <t>listOfAcceptedSenders</t>
+  </si>
+  <si>
+    <t>patricia.ciortin@fwfcompany.com;calin.gandila@fwfcompany.com;diana.sacacian@fwfcompany.com;tudor.cimpean@fwfcompany.com </t>
+  </si>
+  <si>
+    <t>PathOfAttachment</t>
+  </si>
+  <si>
+    <t>C:\Users\AlexandruRotar\Desktop\API Output Report\OutputReport</t>
+  </si>
+  <si>
+    <t>OutputReportPath</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://dog.ceo/api/breeds/image/random </t>
+  </si>
+  <si>
+    <t>dogsAPIURL</t>
+  </si>
+  <si>
+    <t>https://api.thecatapi.com/v1/images/search</t>
+  </si>
+  <si>
+    <t>catsAPIURL</t>
+  </si>
+  <si>
+    <t>C:\Users\AlexandruRotar\Documents\GitHub\API-ANIMALS-PERFORMER\Data\Temp\cat</t>
+  </si>
+  <si>
+    <t>catsPath</t>
+  </si>
+  <si>
+    <t>dogsPath</t>
+  </si>
+  <si>
+    <t>C:\Users\AlexandruRotar\Documents\GitHub\API-ANIMALS-PERFORMER\Data\Temp\dog</t>
   </si>
 </sst>
 </file>
@@ -230,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -241,6 +286,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,8 +603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -643,10 +689,38 @@
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
@@ -1641,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1839,8 +1913,19 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2816,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2864,8 +2949,31 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3866,5 +3974,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit test with attachments sent done
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlexandruRotar\Documents\GitHub\API-ANIMALS-PERFORMER\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F2D4B6-3CA3-42D7-8E0B-568123B90728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F78C6AF0-304A-46C0-BB55-03CB03419D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8445" yWindow="2145" windowWidth="18030" windowHeight="12540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8445" yWindow="2145" windowWidth="18030" windowHeight="12540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -217,6 +217,24 @@
   </si>
   <si>
     <t>C:\Users\AlexandruRotar\Documents\GitHub\API-ANIMALS-PERFORMER\Data\Temp\dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FWFformat </t>
+  </si>
+  <si>
+    <t>fwfcompany.com</t>
+  </si>
+  <si>
+    <t>MailSubject</t>
+  </si>
+  <si>
+    <t>Buna</t>
+  </si>
+  <si>
+    <t>MailBody</t>
+  </si>
+  <si>
+    <t>Priveste!</t>
   </si>
 </sst>
 </file>
@@ -603,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -721,23 +739,41 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2"/>
+    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" s="2"/>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>66</v>
+      </c>
+      <c r="B18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1716,7 +1752,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1927,7 +1963,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2901,7 +2944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>